<commit_message>
Changes for student info export.
</commit_message>
<xml_diff>
--- a/QuickApp/src/QuickApp/wwwroot/ImportStudentInfo.xlsx
+++ b/QuickApp/src/QuickApp/wwwroot/ImportStudentInfo.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>First Name</t>
   </si>
@@ -38,35 +35,133 @@
     <t>PhoneNumber</t>
   </si>
   <si>
-    <t>Anup Shrestha</t>
-  </si>
-  <si>
     <t>bhaktapur</t>
   </si>
   <si>
-    <t>Sagar Dahal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thimi </t>
   </si>
   <si>
-    <t>Sparsha</t>
-  </si>
-  <si>
     <t>Rani kot</t>
   </si>
   <si>
     <t xml:space="preserve">ChannelId </t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Bahadur</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Shrestha</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>anish@gmail.com</t>
+  </si>
+  <si>
+    <t>anis33h@gmail.com</t>
+  </si>
+  <si>
+    <t>ani55sh@gmail.com</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Completed Level</t>
+  </si>
+  <si>
+    <t>Completed Faculty</t>
+  </si>
+  <si>
+    <t>Bachelor</t>
+  </si>
+  <si>
+    <t>BIM</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>MBA</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Interested Faculity</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Phd.</t>
+  </si>
+  <si>
+    <t>BSCIT</t>
+  </si>
+  <si>
+    <t>Suba</t>
+  </si>
+  <si>
+    <t>Sabina</t>
+  </si>
+  <si>
+    <t>Siprata</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Lalitpur</t>
+  </si>
+  <si>
+    <t>Shusil</t>
+  </si>
+  <si>
+    <t>Thapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magar </t>
+  </si>
+  <si>
+    <t>Thankot</t>
+  </si>
+  <si>
+    <t>ani323sh@gmail.com0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,13 +184,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,88 +472,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>443</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>9800909090</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>9800909090</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>88</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>224</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
+      <c r="G3">
         <v>9989898080</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3">
+        <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>225</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
+      <c r="G4">
         <v>980980878</v>
       </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5">
+        <v>214214214</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>